<commit_message>
Att preliminary round complete
</commit_message>
<xml_diff>
--- a/2025 FIVB Men's Volleyball World Championship.xlsx
+++ b/2025 FIVB Men's Volleyball World Championship.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A9E86A1-23A4-461C-916E-3E874DCD86AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D05B025F-9BA3-4D6C-A32B-EA86B4708C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="1" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
   </bookViews>
   <sheets>
     <sheet name="Dummy" sheetId="2" state="hidden" r:id="rId1"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="B3" s="1">
         <f>RANK(F3,$F$3:$F$6)+SUM(T3:W3)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
         <f>Preliminary!AB6</f>
@@ -2414,11 +2414,11 @@
       </c>
       <c r="D3" s="1">
         <f>SUM(H3*3,I3*3,J3*2,K3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
         <f>F3+G3</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C3)</f>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="G3" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C3,Preliminary!AI:AI)</f>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C3,Preliminary!AS:AS)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C3,Preliminary!AT:AT)</f>
@@ -2454,27 +2454,27 @@
       </c>
       <c r="N3" s="1">
         <f>SUMIF(Preliminary!AE:AE,C3,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C3,Preliminary!AQ:AQ)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1">
         <f>SUMIF(Preliminary!AE:AE,C3,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C3,Preliminary!AR:AR)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P3" s="4">
         <f>IFERROR((N3/O3)*1000,"MAX")</f>
-        <v>750</v>
+        <v>714.28571428571433</v>
       </c>
       <c r="Q3" s="1">
         <f>SUMIF(Preliminary!AE:AE,C3,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C3,Preliminary!AV:AV)</f>
-        <v>155</v>
+        <v>269</v>
       </c>
       <c r="R3" s="1">
         <f>SUMIF(Preliminary!AE:AE,C3,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C3,Preliminary!AW:AW)</f>
-        <v>169</v>
+        <v>279</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" ref="S3:S20" si="0">IFERROR((Q3/R3)*1000,"MAX")</f>
-        <v>917.15976331360946</v>
+        <v>964.15770609318997</v>
       </c>
       <c r="T3" s="1">
         <f>SUMPRODUCT(($F$3:$F$6=F3)*($D$3:$D$6&gt;D3))</f>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="U3" s="1">
         <f>SUMPRODUCT(($F$3:$F$6=F3)*($D$3:$D$6=D3)*($P$3:$P$6&gt;P3))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1">
         <f>SUMPRODUCT(($F$3:$F$6=F3)*($D$3:$D$6=D3)*($P$3:$P$6=P3)*($S$3:$S$6&gt;S3))</f>
@@ -2508,15 +2508,15 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D20" si="1">SUM(H4*3,I4*3,J4*2,K4)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ref="E4:E20" si="2">F4+G4</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C4)</f>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="J4" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C4,Preliminary!AK:AK)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C4,Preliminary!AS:AS)</f>
@@ -2548,35 +2548,35 @@
       </c>
       <c r="N4" s="1">
         <f>SUMIF(Preliminary!AE:AE,C4,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C4,Preliminary!AQ:AQ)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O4" s="1">
         <f>SUMIF(Preliminary!AE:AE,C4,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C4,Preliminary!AR:AR)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4:P20" si="3">IFERROR((N4/O4)*1000,"MAX")</f>
-        <v>1000</v>
+        <v>1166.6666666666667</v>
       </c>
       <c r="Q4" s="1">
         <f>SUMIF(Preliminary!AE:AE,C4,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C4,Preliminary!AV:AV)</f>
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="R4" s="1">
         <f>SUMIF(Preliminary!AE:AE,C4,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C4,Preliminary!AW:AW)</f>
-        <v>175</v>
+        <v>289</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="0"/>
-        <v>1045.7142857142858</v>
+        <v>1013.840830449827</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" ref="T4:T6" si="4">SUMPRODUCT(($F$3:$F$6=F4)*($D$3:$D$6&gt;D4))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1">
         <f t="shared" ref="U4:U6" si="5">SUMPRODUCT(($F$3:$F$6=F4)*($D$3:$D$6=D4)*($P$3:$P$6&gt;P4))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <f t="shared" ref="V4:V6" si="6">SUMPRODUCT(($F$3:$F$6=F4)*($D$3:$D$6=D4)*($P$3:$P$6=P4)*($S$3:$S$6&gt;S4))</f>
@@ -2594,7 +2594,7 @@
       <c r="A5" s="55"/>
       <c r="B5" s="1">
         <f>RANK(F5,$F$3:$F$6)+SUM(T5:W5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
         <f>Preliminary!AB8</f>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C5)</f>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G5" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C5,Preliminary!AI:AI)</f>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="M5" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C5,Preliminary!AU:AU)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="1">
         <f>SUMIF(Preliminary!AE:AE,C5,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C5,Preliminary!AQ:AQ)</f>
@@ -2646,35 +2646,35 @@
       </c>
       <c r="O5" s="1">
         <f>SUMIF(Preliminary!AE:AE,C5,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C5,Preliminary!AR:AR)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="Q5" s="1">
         <f>SUMIF(Preliminary!AE:AE,C5,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C5,Preliminary!AV:AV)</f>
-        <v>185</v>
+        <v>244</v>
       </c>
       <c r="R5" s="1">
         <f>SUMIF(Preliminary!AE:AE,C5,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C5,Preliminary!AW:AW)</f>
-        <v>187</v>
+        <v>262</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="0"/>
-        <v>989.30481283422455</v>
+        <v>931.29770992366412</v>
       </c>
       <c r="T5" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" s="1">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" s="1">
         <f t="shared" si="7"/>
@@ -2696,15 +2696,15 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C6)</f>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="H6" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C6,Preliminary!AI:AI)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C6,Preliminary!AJ:AJ)</f>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="N6" s="1">
         <f>SUMIF(Preliminary!AE:AE,C6,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C6,Preliminary!AQ:AQ)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O6" s="1">
         <f>SUMIF(Preliminary!AE:AE,C6,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C6,Preliminary!AR:AR)</f>
@@ -2744,19 +2744,19 @@
       </c>
       <c r="P6" s="4">
         <f t="shared" si="3"/>
-        <v>1333.3333333333333</v>
+        <v>2333.3333333333335</v>
       </c>
       <c r="Q6" s="1">
         <f>SUMIF(Preliminary!AE:AE,C6,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C6,Preliminary!AV:AV)</f>
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="R6" s="1">
         <f>SUMIF(Preliminary!AE:AE,C6,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C6,Preliminary!AW:AW)</f>
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="0"/>
-        <v>1052.9801324503312</v>
+        <v>1114.2857142857142</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" si="4"/>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="B11" s="1">
         <f>RANK(F11,$F$11:$F$14)+SUM(T11:W11)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f>Preliminary!AB22</f>
@@ -3170,11 +3170,11 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C11)</f>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="G11" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C11,Preliminary!AI:AI)</f>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="K11" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C11,Preliminary!AS:AS)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C11,Preliminary!AT:AT)</f>
@@ -3210,27 +3210,27 @@
       </c>
       <c r="N11" s="1">
         <f>SUMIF(Preliminary!AE:AE,C11,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C11,Preliminary!AQ:AQ)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O11" s="1">
         <f>SUMIF(Preliminary!AE:AE,C11,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C11,Preliminary!AR:AR)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="3"/>
-        <v>1666.6666666666667</v>
+        <v>1166.6666666666667</v>
       </c>
       <c r="Q11" s="1">
         <f>SUMIF(Preliminary!AE:AE,C11,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C11,Preliminary!AV:AV)</f>
-        <v>180</v>
+        <v>291</v>
       </c>
       <c r="R11" s="1">
         <f>SUMIF(Preliminary!AE:AE,C11,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C11,Preliminary!AW:AW)</f>
-        <v>153</v>
+        <v>262</v>
       </c>
       <c r="S11" s="4">
         <f t="shared" si="0"/>
-        <v>1176.4705882352941</v>
+        <v>1110.6870229007632</v>
       </c>
       <c r="T11" s="1">
         <f>SUMPRODUCT(($F$11:$F$14=F11)*($D$11:$D$14&gt;D11))</f>
@@ -3264,15 +3264,15 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C12)</f>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="J12" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C12,Preliminary!AK:AK)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C12,Preliminary!AS:AS)</f>
@@ -3304,27 +3304,27 @@
       </c>
       <c r="N12" s="1">
         <f>SUMIF(Preliminary!AE:AE,C12,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C12,Preliminary!AQ:AQ)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O12" s="1">
         <f>SUMIF(Preliminary!AE:AE,C12,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C12,Preliminary!AR:AR)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="Q12" s="1">
         <f>SUMIF(Preliminary!AE:AE,C12,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C12,Preliminary!AV:AV)</f>
-        <v>200</v>
+        <v>309</v>
       </c>
       <c r="R12" s="1">
         <f>SUMIF(Preliminary!AE:AE,C12,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C12,Preliminary!AW:AW)</f>
-        <v>191</v>
+        <v>302</v>
       </c>
       <c r="S12" s="4">
         <f t="shared" si="0"/>
-        <v>1047.1204188481674</v>
+        <v>1023.1788079470199</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" ref="T12:T14" si="14">SUMPRODUCT(($F$11:$F$14=F12)*($D$11:$D$14&gt;D12))</f>
@@ -3350,7 +3350,7 @@
       <c r="A13" s="55"/>
       <c r="B13" s="1">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="str">
         <f>Preliminary!AB24</f>
@@ -3358,15 +3358,15 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C13)</f>
@@ -3378,7 +3378,7 @@
       </c>
       <c r="I13" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C13,Preliminary!AJ:AJ)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C13,Preliminary!AK:AK)</f>
@@ -3398,31 +3398,31 @@
       </c>
       <c r="N13" s="1">
         <f>SUMIF(Preliminary!AE:AE,C13,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C13,Preliminary!AQ:AQ)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O13" s="1">
         <f>SUMIF(Preliminary!AE:AE,C13,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C13,Preliminary!AR:AR)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1333.3333333333333</v>
       </c>
       <c r="Q13" s="1">
         <f>SUMIF(Preliminary!AE:AE,C13,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C13,Preliminary!AV:AV)</f>
-        <v>212</v>
+        <v>304</v>
       </c>
       <c r="R13" s="1">
         <f>SUMIF(Preliminary!AE:AE,C13,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C13,Preliminary!AW:AW)</f>
-        <v>207</v>
+        <v>294</v>
       </c>
       <c r="S13" s="4">
         <f t="shared" si="0"/>
-        <v>1024.1545893719808</v>
+        <v>1034.0136054421769</v>
       </c>
       <c r="T13" s="1">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1">
         <f t="shared" si="15"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C14)</f>
@@ -3464,7 +3464,7 @@
       </c>
       <c r="G14" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C14,Preliminary!AI:AI)</f>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L14" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C14,Preliminary!AT:AT)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C14,Preliminary!AU:AU)</f>
@@ -3492,27 +3492,27 @@
       </c>
       <c r="N14" s="1">
         <f>SUMIF(Preliminary!AE:AE,C14,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C14,Preliminary!AQ:AQ)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="1">
         <f>SUMIF(Preliminary!AE:AE,C14,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C14,Preliminary!AR:AR)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" si="3"/>
-        <v>166.66666666666666</v>
+        <v>222.2222222222222</v>
       </c>
       <c r="Q14" s="1">
         <f>SUMIF(Preliminary!AE:AE,C14,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C14,Preliminary!AV:AV)</f>
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="R14" s="1">
         <f>SUMIF(Preliminary!AE:AE,C14,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C14,Preliminary!AW:AW)</f>
-        <v>173</v>
+        <v>265</v>
       </c>
       <c r="S14" s="4">
         <f t="shared" si="0"/>
-        <v>763.00578034682076</v>
+        <v>826.41509433962267</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="14"/>
@@ -4304,15 +4304,15 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C23)</f>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C23,Preliminary!AI:AI)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C23,Preliminary!AJ:AJ)</f>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="N23" s="1">
         <f>SUMIF(Preliminary!AE:AE,C23,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C23,Preliminary!AQ:AQ)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O23" s="1">
         <f>SUMIF(Preliminary!AE:AE,C23,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C23,Preliminary!AR:AR)</f>
@@ -4352,19 +4352,19 @@
       </c>
       <c r="P23" s="4">
         <f t="shared" si="26"/>
-        <v>1666.6666666666667</v>
+        <v>2666.6666666666665</v>
       </c>
       <c r="Q23" s="1">
         <f>SUMIF(Preliminary!AE:AE,C23,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C23,Preliminary!AV:AV)</f>
-        <v>181</v>
+        <v>256</v>
       </c>
       <c r="R23" s="1">
         <f>SUMIF(Preliminary!AE:AE,C23,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C23,Preliminary!AW:AW)</f>
-        <v>160</v>
+        <v>221</v>
       </c>
       <c r="S23" s="4">
         <f t="shared" si="27"/>
-        <v>1131.25</v>
+        <v>1158.3710407239821</v>
       </c>
       <c r="T23" s="1">
         <f>SUMPRODUCT(($F$23:$F$26=F23)*($D$23:$D$26&gt;D23))</f>
@@ -4402,7 +4402,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C24)</f>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="G24" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C24)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C24,Preliminary!AI:AI)</f>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="M24" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C24,Preliminary!AU:AU)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N24" s="1">
         <f>SUMIF(Preliminary!AE:AE,C24,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C24,Preliminary!AQ:AQ)</f>
@@ -4442,27 +4442,27 @@
       </c>
       <c r="O24" s="1">
         <f>SUMIF(Preliminary!AE:AE,C24,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C24,Preliminary!AR:AR)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="26"/>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q24" s="1">
         <f>SUMIF(Preliminary!AE:AE,C24,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C24,Preliminary!AV:AV)</f>
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="R24" s="1">
         <f>SUMIF(Preliminary!AE:AE,C24,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C24,Preliminary!AW:AW)</f>
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="27"/>
-        <v>1130.4347826086955</v>
+        <v>1005.2631578947369</v>
       </c>
       <c r="T24" s="1">
         <f>SUMPRODUCT(($F$23:$F$26=F24)*($D$23:$D$26&gt;D24))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24" s="1">
         <f>SUMPRODUCT(($F$23:$F$26=F24)*($D$23:$D$26=D24)*($P$23:$P$26&gt;P24))</f>
@@ -4492,15 +4492,15 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="24"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C25)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C25)</f>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C25,Preliminary!AI:AI)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C25,Preliminary!AJ:AJ)</f>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="N25" s="1">
         <f>SUMIF(Preliminary!AE:AE,C25,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C25,Preliminary!AQ:AQ)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O25" s="1">
         <f>SUMIF(Preliminary!AE:AE,C25,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C25,Preliminary!AR:AR)</f>
@@ -4540,19 +4540,19 @@
       </c>
       <c r="P25" s="4">
         <f t="shared" si="26"/>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="Q25" s="1">
         <f>SUMIF(Preliminary!AE:AE,C25,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C25,Preliminary!AV:AV)</f>
-        <v>183</v>
+        <v>258</v>
       </c>
       <c r="R25" s="1">
         <f>SUMIF(Preliminary!AE:AE,C25,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C25,Preliminary!AW:AW)</f>
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="27"/>
-        <v>1136.6459627329193</v>
+        <v>1200</v>
       </c>
       <c r="T25" s="1">
         <f>SUMPRODUCT(($F$23:$F$26=F25)*($D$23:$D$26&gt;D25))</f>
@@ -4590,7 +4590,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C26)</f>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="G26" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C26)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C26,Preliminary!AI:AI)</f>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="M26" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C26,Preliminary!AU:AU)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N26" s="1">
         <f>SUMIF(Preliminary!AE:AE,C26,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C26,Preliminary!AQ:AQ)</f>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="O26" s="1">
         <f>SUMIF(Preliminary!AE:AE,C26,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C26,Preliminary!AR:AR)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P26" s="4">
         <f t="shared" si="26"/>
@@ -4638,15 +4638,15 @@
       </c>
       <c r="Q26" s="1">
         <f>SUMIF(Preliminary!AE:AE,C26,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C26,Preliminary!AV:AV)</f>
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="R26" s="1">
         <f>SUMIF(Preliminary!AE:AE,C26,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C26,Preliminary!AW:AW)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="S26" s="4">
         <f t="shared" si="27"/>
-        <v>613.33333333333326</v>
+        <v>648.8888888888888</v>
       </c>
       <c r="T26" s="1">
         <f>SUMPRODUCT(($F$23:$F$26=F26)*($D$23:$D$26&gt;D26))</f>
@@ -5052,7 +5052,7 @@
       </c>
       <c r="B31" s="1">
         <f>RANK(F31,$F$31:$F$34)+SUM(T31:W31)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" t="str">
         <f>Preliminary!AB62</f>
@@ -5064,7 +5064,7 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C31)</f>
@@ -5072,7 +5072,7 @@
       </c>
       <c r="G31" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C31,Preliminary!AI:AI)</f>
@@ -5096,7 +5096,7 @@
       </c>
       <c r="M31" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C31,Preliminary!AU:AU)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="1">
         <f>SUMIF(Preliminary!AE:AE,C31,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C31,Preliminary!AQ:AQ)</f>
@@ -5104,23 +5104,23 @@
       </c>
       <c r="O31" s="1">
         <f>SUMIF(Preliminary!AE:AE,C31,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C31,Preliminary!AR:AR)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P31" s="4">
         <f t="shared" si="26"/>
-        <v>6000</v>
+        <v>1500</v>
       </c>
       <c r="Q31" s="1">
         <f>SUMIF(Preliminary!AE:AE,C31,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C31,Preliminary!AV:AV)</f>
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="R31" s="1">
         <f>SUMIF(Preliminary!AE:AE,C31,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C31,Preliminary!AW:AW)</f>
-        <v>142</v>
+        <v>217</v>
       </c>
       <c r="S31" s="4">
         <f t="shared" si="27"/>
-        <v>1190.1408450704225</v>
+        <v>1073.7327188940092</v>
       </c>
       <c r="T31" s="1">
         <f>SUMPRODUCT(($F$31:$F$34=F31)*($D$31:$D$34&gt;D31))</f>
@@ -5128,7 +5128,7 @@
       </c>
       <c r="U31" s="1">
         <f>SUMPRODUCT(($F$31:$F$34=F31)*($D$31:$D$34=D31)*($P$31:$P$34&gt;P31))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V31" s="1">
         <f>SUMPRODUCT(($F$31:$F$34=F31)*($D$31:$D$34=D31)*($P$31:$P$34=P31)*($S$31:$S$34&gt;S31))</f>
@@ -5146,7 +5146,7 @@
       <c r="A32" s="55"/>
       <c r="B32" s="1">
         <f t="shared" ref="B32:B34" si="34">RANK(F32,$F$31:$F$34)+SUM(T32:W32)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="str">
         <f>Preliminary!AB63</f>
@@ -5154,15 +5154,15 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C32)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C32)</f>
@@ -5170,7 +5170,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C32,Preliminary!AI:AI)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C32,Preliminary!AJ:AJ)</f>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="N32" s="1">
         <f>SUMIF(Preliminary!AE:AE,C32,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C32,Preliminary!AQ:AQ)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O32" s="1">
         <f>SUMIF(Preliminary!AE:AE,C32,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C32,Preliminary!AR:AR)</f>
@@ -5202,19 +5202,19 @@
       </c>
       <c r="P32" s="4">
         <f t="shared" si="26"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="Q32" s="1">
         <f>SUMIF(Preliminary!AE:AE,C32,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C32,Preliminary!AV:AV)</f>
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="R32" s="1">
         <f>SUMIF(Preliminary!AE:AE,C32,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C32,Preliminary!AW:AW)</f>
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="S32" s="4">
         <f t="shared" si="27"/>
-        <v>1035.9712230215828</v>
+        <v>1078.8177339901476</v>
       </c>
       <c r="T32" s="1">
         <f t="shared" ref="T32:T34" si="35">SUMPRODUCT(($F$31:$F$34=F32)*($D$31:$D$34&gt;D32))</f>
@@ -5240,7 +5240,7 @@
       <c r="A33" s="55"/>
       <c r="B33" s="1">
         <f t="shared" si="34"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="str">
         <f>Preliminary!AB64</f>
@@ -5248,15 +5248,15 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C33)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C33)</f>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C33,Preliminary!AI:AI)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C33,Preliminary!AJ:AJ)</f>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="N33" s="1">
         <f>SUMIF(Preliminary!AE:AE,C33,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C33,Preliminary!AQ:AQ)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O33" s="1">
         <f>SUMIF(Preliminary!AE:AE,C33,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C33,Preliminary!AR:AR)</f>
@@ -5296,19 +5296,19 @@
       </c>
       <c r="P33" s="4">
         <f t="shared" si="26"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="Q33" s="1">
         <f>SUMIF(Preliminary!AE:AE,C33,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C33,Preliminary!AV:AV)</f>
-        <v>126</v>
+        <v>202</v>
       </c>
       <c r="R33" s="1">
         <f>SUMIF(Preliminary!AE:AE,C33,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C33,Preliminary!AW:AW)</f>
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="S33" s="4">
         <f t="shared" si="27"/>
-        <v>900</v>
+        <v>1004.9751243781095</v>
       </c>
       <c r="T33" s="1">
         <f t="shared" si="35"/>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" s="1">
         <f>COUNTIF(Preliminary!AE:AE,Dummy!C34)</f>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="G34" s="1">
         <f>COUNTIF(Preliminary!AO:AO,Dummy!C34)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H34" s="1">
         <f>SUMIF(Preliminary!$AE:$AE,Dummy!$C34,Preliminary!AI:AI)</f>
@@ -5378,7 +5378,7 @@
       </c>
       <c r="M34" s="1">
         <f>SUMIF(Preliminary!$AO:$AO,Dummy!$C34,Preliminary!AU:AU)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N34" s="1">
         <f>SUMIF(Preliminary!AE:AE,C34,Preliminary!AG:AG)+SUMIF(Preliminary!AO:AO,C34,Preliminary!AQ:AQ)</f>
@@ -5386,23 +5386,23 @@
       </c>
       <c r="O34" s="1">
         <f>SUMIF(Preliminary!AE:AE,C34,Preliminary!AH:AH)+SUMIF(Preliminary!AO:AO,C34,Preliminary!AR:AR)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P34" s="4">
         <f t="shared" si="26"/>
-        <v>166.66666666666666</v>
+        <v>111.1111111111111</v>
       </c>
       <c r="Q34" s="1">
         <f>SUMIF(Preliminary!AE:AE,C34,Preliminary!AL:AL)+SUMIF(Preliminary!AO:AO,C34,Preliminary!AV:AV)</f>
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="R34" s="1">
         <f>SUMIF(Preliminary!AE:AE,C34,Preliminary!AM:AM)+SUMIF(Preliminary!AO:AO,C34,Preliminary!AW:AW)</f>
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="S34" s="4">
         <f t="shared" si="27"/>
-        <v>895.95375722543361</v>
+        <v>867.46987951807228</v>
       </c>
       <c r="T34" s="1">
         <f t="shared" si="35"/>
@@ -5448,8 +5448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842A5577-D33C-4D22-A376-2229D9D229A5}">
   <dimension ref="B2:BR67"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6169,15 +6169,15 @@
       </c>
       <c r="AZ7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BA7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,6,FALSE)</f>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="BD7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,7,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,8,FALSE)</f>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="BJ7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,13,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BK7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,14,FALSE)</f>
@@ -6217,19 +6217,19 @@
       </c>
       <c r="BL7" s="52">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,15,FALSE)</f>
-        <v>1333.3333333333333</v>
+        <v>2333.3333333333335</v>
       </c>
       <c r="BM7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,16,FALSE)</f>
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="BN7" s="50">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,17,FALSE)</f>
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="BO7" s="52">
         <f>VLOOKUP($AX7,Dummy!$B$3:$S$6,18,FALSE)</f>
-        <v>1052.9801324503312</v>
+        <v>1114.2857142857142</v>
       </c>
     </row>
     <row r="8" spans="2:67" x14ac:dyDescent="0.25">
@@ -6396,15 +6396,15 @@
       </c>
       <c r="AZ8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,3,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BA8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,6,FALSE)</f>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="BF8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,10,FALSE)</f>
@@ -6436,27 +6436,27 @@
       </c>
       <c r="BJ8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,13,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BK8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,14,FALSE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BL8" s="52">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,15,FALSE)</f>
-        <v>1000</v>
+        <v>1166.6666666666667</v>
       </c>
       <c r="BM8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,16,FALSE)</f>
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="BN8" s="50">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,17,FALSE)</f>
-        <v>175</v>
+        <v>289</v>
       </c>
       <c r="BO8" s="52">
         <f>VLOOKUP($AX8,Dummy!$B$3:$S$6,18,FALSE)</f>
-        <v>1045.7142857142858</v>
+        <v>1013.840830449827</v>
       </c>
     </row>
     <row r="9" spans="2:67" x14ac:dyDescent="0.25">
@@ -6619,15 +6619,15 @@
       </c>
       <c r="AY9" s="51" t="str">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,2,FALSE)</f>
-        <v>Egypt</v>
+        <v>Philippines</v>
       </c>
       <c r="AZ9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,3,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,5,FALSE)</f>
@@ -6635,7 +6635,7 @@
       </c>
       <c r="BC9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,7,FALSE)</f>
@@ -6651,39 +6651,39 @@
       </c>
       <c r="BG9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,11,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,12,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,13,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BK9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,14,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BL9" s="52">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,15,FALSE)</f>
-        <v>1000</v>
+        <v>714.28571428571433</v>
       </c>
       <c r="BM9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,16,FALSE)</f>
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="BN9" s="50">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,17,FALSE)</f>
-        <v>187</v>
+        <v>279</v>
       </c>
       <c r="BO9" s="52">
         <f>VLOOKUP($AX9,Dummy!$B$3:$S$6,18,FALSE)</f>
-        <v>989.30481283422455</v>
+        <v>964.15770609318997</v>
       </c>
     </row>
     <row r="10" spans="2:67" x14ac:dyDescent="0.25">
@@ -6694,30 +6694,46 @@
         <f>AB8</f>
         <v>Egypt</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="48">
+        <v>0</v>
+      </c>
       <c r="E10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="47"/>
+      <c r="F10" s="47">
+        <v>3</v>
+      </c>
       <c r="G10" s="25" t="str">
         <f>AB9</f>
         <v>Tunisia</v>
       </c>
-      <c r="H10" s="28"/>
+      <c r="H10" s="28">
+        <v>19</v>
+      </c>
       <c r="I10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="28"/>
+      <c r="J10" s="30">
+        <v>25</v>
+      </c>
+      <c r="K10" s="28">
+        <v>18</v>
+      </c>
       <c r="L10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="28"/>
+      <c r="M10" s="30">
+        <v>25</v>
+      </c>
+      <c r="N10" s="28">
+        <v>22</v>
+      </c>
       <c r="O10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="30"/>
+      <c r="P10" s="30">
+        <v>25</v>
+      </c>
       <c r="Q10" s="28"/>
       <c r="R10" s="29" t="s">
         <v>0</v>
@@ -6730,30 +6746,30 @@
       <c r="V10" s="30"/>
       <c r="W10" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="X10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y10" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AE10" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>Tunisia</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="6"/>
@@ -6761,7 +6777,7 @@
       </c>
       <c r="AI10" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10" s="12">
         <f t="shared" si="8"/>
@@ -6773,19 +6789,19 @@
       </c>
       <c r="AL10" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AM10" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AO10" s="12">
+        <v>59</v>
+      </c>
+      <c r="AO10" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>Egypt</v>
       </c>
       <c r="AP10" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ10" s="12">
         <f t="shared" si="14"/>
@@ -6793,7 +6809,7 @@
       </c>
       <c r="AR10" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS10" s="12">
         <f t="shared" si="16"/>
@@ -6805,22 +6821,22 @@
       </c>
       <c r="AU10" s="12">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV10" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AW10" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AX10" s="50">
         <v>4</v>
       </c>
       <c r="AY10" s="51" t="str">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,2,FALSE)</f>
-        <v>Philippines</v>
+        <v>Egypt</v>
       </c>
       <c r="AZ10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,3,FALSE)</f>
@@ -6828,7 +6844,7 @@
       </c>
       <c r="BA10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,5,FALSE)</f>
@@ -6836,7 +6852,7 @@
       </c>
       <c r="BC10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,7,FALSE)</f>
@@ -6856,7 +6872,7 @@
       </c>
       <c r="BH10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,11,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,12,FALSE)</f>
@@ -6864,27 +6880,27 @@
       </c>
       <c r="BJ10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,13,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BK10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,14,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BL10" s="52">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,15,FALSE)</f>
-        <v>750</v>
+        <v>571.42857142857144</v>
       </c>
       <c r="BM10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,16,FALSE)</f>
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="BN10" s="50">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,17,FALSE)</f>
-        <v>169</v>
+        <v>262</v>
       </c>
       <c r="BO10" s="52">
         <f>VLOOKUP($AX10,Dummy!$B$3:$S$6,18,FALSE)</f>
-        <v>917.15976331360946</v>
+        <v>931.29770992366412</v>
       </c>
     </row>
     <row r="11" spans="2:67" x14ac:dyDescent="0.25">
@@ -6895,70 +6911,94 @@
         <f>AB6</f>
         <v>Philippines</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="48">
+        <v>2</v>
+      </c>
       <c r="E11" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="47"/>
+      <c r="F11" s="47">
+        <v>3</v>
+      </c>
       <c r="G11" s="25" t="str">
         <f>AB7</f>
         <v>Iran</v>
       </c>
-      <c r="H11" s="28"/>
+      <c r="H11" s="28">
+        <v>25</v>
+      </c>
       <c r="I11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="28"/>
+      <c r="J11" s="30">
+        <v>21</v>
+      </c>
+      <c r="K11" s="28">
+        <v>21</v>
+      </c>
       <c r="L11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="28"/>
+      <c r="M11" s="30">
+        <v>25</v>
+      </c>
+      <c r="N11" s="28">
+        <v>25</v>
+      </c>
       <c r="O11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="28"/>
+      <c r="P11" s="30">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>23</v>
+      </c>
       <c r="R11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="30"/>
-      <c r="T11" s="28"/>
+      <c r="S11" s="30">
+        <v>25</v>
+      </c>
+      <c r="T11" s="28">
+        <v>20</v>
+      </c>
       <c r="U11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="V11" s="30"/>
+      <c r="V11" s="30">
+        <v>22</v>
+      </c>
       <c r="W11" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="X11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y11" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="12">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>Iran</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI11" s="12">
         <f t="shared" si="7"/>
@@ -6970,35 +7010,35 @@
       </c>
       <c r="AK11" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL11" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AM11" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AO11" s="12">
+        <v>114</v>
+      </c>
+      <c r="AO11" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>Philippines</v>
       </c>
       <c r="AP11" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ11" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR11" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS11" s="12">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT11" s="12">
         <f t="shared" si="17"/>
@@ -7010,15 +7050,15 @@
       </c>
       <c r="AV11" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="AW11" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="BA11" s="26">
         <f>SUM(BA7:BA10)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9043,15 +9083,15 @@
       </c>
       <c r="AZ23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,3,FALSE)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BA23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,6,FALSE)</f>
@@ -9067,7 +9107,7 @@
       </c>
       <c r="BF23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BG23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,10,FALSE)</f>
@@ -9083,27 +9123,27 @@
       </c>
       <c r="BJ23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,13,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BK23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,14,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BL23" s="52">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,15,FALSE)</f>
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="BM23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,16,FALSE)</f>
-        <v>200</v>
+        <v>309</v>
       </c>
       <c r="BN23" s="50">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,17,FALSE)</f>
-        <v>191</v>
+        <v>302</v>
       </c>
       <c r="BO23" s="52">
         <f>VLOOKUP($AX23,Dummy!$B$11:$S$14,18,FALSE)</f>
-        <v>1047.1204188481674</v>
+        <v>1023.1788079470199</v>
       </c>
     </row>
     <row r="24" spans="2:67" x14ac:dyDescent="0.25">
@@ -9266,19 +9306,19 @@
       </c>
       <c r="AY24" s="51" t="str">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,2,FALSE)</f>
-        <v>France</v>
+        <v>Finland</v>
       </c>
       <c r="AZ24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,3,FALSE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BA24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,6,FALSE)</f>
@@ -9286,15 +9326,15 @@
       </c>
       <c r="BD24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,7,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,8,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,10,FALSE)</f>
@@ -9310,27 +9350,27 @@
       </c>
       <c r="BJ24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,13,FALSE)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BK24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,14,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BL24" s="52">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,15,FALSE)</f>
-        <v>1666.6666666666667</v>
+        <v>1333.3333333333333</v>
       </c>
       <c r="BM24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,16,FALSE)</f>
-        <v>180</v>
+        <v>304</v>
       </c>
       <c r="BN24" s="50">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,17,FALSE)</f>
-        <v>153</v>
+        <v>294</v>
       </c>
       <c r="BO24" s="52">
         <f>VLOOKUP($AX24,Dummy!$B$11:$S$14,18,FALSE)</f>
-        <v>1176.4705882352941</v>
+        <v>1034.0136054421769</v>
       </c>
     </row>
     <row r="25" spans="2:67" x14ac:dyDescent="0.25">
@@ -9497,15 +9537,15 @@
       </c>
       <c r="AY25" s="51" t="str">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,2,FALSE)</f>
-        <v>Finland</v>
+        <v>France</v>
       </c>
       <c r="AZ25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,3,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BA25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,5,FALSE)</f>
@@ -9513,11 +9553,11 @@
       </c>
       <c r="BC25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,8,FALSE)</f>
@@ -9525,11 +9565,11 @@
       </c>
       <c r="BF25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,9,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,10,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BH25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,11,FALSE)</f>
@@ -9541,27 +9581,27 @@
       </c>
       <c r="BJ25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,13,FALSE)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="BK25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,14,FALSE)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BL25" s="52">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,15,FALSE)</f>
-        <v>1000</v>
+        <v>1166.6666666666667</v>
       </c>
       <c r="BM25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,16,FALSE)</f>
-        <v>212</v>
+        <v>291</v>
       </c>
       <c r="BN25" s="50">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,17,FALSE)</f>
-        <v>207</v>
+        <v>262</v>
       </c>
       <c r="BO25" s="52">
         <f>VLOOKUP($AX25,Dummy!$B$11:$S$14,18,FALSE)</f>
-        <v>1024.1545893719808</v>
+        <v>1110.6870229007632</v>
       </c>
     </row>
     <row r="26" spans="2:67" x14ac:dyDescent="0.25">
@@ -9572,35 +9612,55 @@
         <f>AB24</f>
         <v>Finland</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="48">
+        <v>3</v>
+      </c>
       <c r="E26" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="47"/>
+      <c r="F26" s="47">
+        <v>1</v>
+      </c>
       <c r="G26" s="25" t="str">
         <f>AB25</f>
         <v>South Korea</v>
       </c>
-      <c r="H26" s="28"/>
+      <c r="H26" s="28">
+        <v>25</v>
+      </c>
       <c r="I26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="28"/>
+      <c r="J26" s="30">
+        <v>18</v>
+      </c>
+      <c r="K26" s="28">
+        <v>25</v>
+      </c>
       <c r="L26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M26" s="30"/>
-      <c r="N26" s="28"/>
+      <c r="M26" s="30">
+        <v>23</v>
+      </c>
+      <c r="N26" s="28">
+        <v>17</v>
+      </c>
       <c r="O26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="28"/>
+      <c r="P26" s="30">
+        <v>25</v>
+      </c>
+      <c r="Q26" s="28">
+        <v>25</v>
+      </c>
       <c r="R26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S26" s="30"/>
+      <c r="S26" s="30">
+        <v>21</v>
+      </c>
       <c r="T26" s="28"/>
       <c r="U26" s="29" t="s">
         <v>0</v>
@@ -9608,34 +9668,34 @@
       <c r="V26" s="30"/>
       <c r="W26" s="31">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="X26" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y26" s="32">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="AD26" s="12">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="AE26" s="12">
+        <v>4</v>
+      </c>
+      <c r="AE26" s="12" t="str">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>Finland</v>
       </c>
       <c r="AF26" s="12">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG26" s="12">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH26" s="12">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI26" s="12">
         <f t="shared" si="47"/>
@@ -9643,7 +9703,7 @@
       </c>
       <c r="AJ26" s="12">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK26" s="12">
         <f t="shared" si="49"/>
@@ -9651,27 +9711,27 @@
       </c>
       <c r="AL26" s="12">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="AM26" s="12">
         <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="AO26" s="12">
+        <v>87</v>
+      </c>
+      <c r="AO26" s="12" t="str">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>South Korea</v>
       </c>
       <c r="AP26" s="12">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ26" s="12">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR26" s="12">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS26" s="12">
         <f t="shared" si="56"/>
@@ -9679,7 +9739,7 @@
       </c>
       <c r="AT26" s="12">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU26" s="12">
         <f t="shared" si="58"/>
@@ -9687,11 +9747,11 @@
       </c>
       <c r="AV26" s="12">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="AW26" s="12">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="AX26" s="50">
         <v>4</v>
@@ -9706,7 +9766,7 @@
       </c>
       <c r="BA26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,5,FALSE)</f>
@@ -9714,7 +9774,7 @@
       </c>
       <c r="BC26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,6,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,7,FALSE)</f>
@@ -9734,7 +9794,7 @@
       </c>
       <c r="BH26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,11,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BI26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,12,FALSE)</f>
@@ -9742,27 +9802,27 @@
       </c>
       <c r="BJ26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,13,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BK26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,14,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BL26" s="52">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,15,FALSE)</f>
-        <v>166.66666666666666</v>
+        <v>222.2222222222222</v>
       </c>
       <c r="BM26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,16,FALSE)</f>
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="BN26" s="50">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,17,FALSE)</f>
-        <v>173</v>
+        <v>265</v>
       </c>
       <c r="BO26" s="52">
         <f>VLOOKUP($AX26,Dummy!$B$11:$S$14,18,FALSE)</f>
-        <v>763.00578034682076</v>
+        <v>826.41509433962267</v>
       </c>
     </row>
     <row r="27" spans="2:67" x14ac:dyDescent="0.25">
@@ -9773,70 +9833,94 @@
         <f>AB22</f>
         <v>France</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="48">
+        <v>2</v>
+      </c>
       <c r="E27" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F27" s="47"/>
+      <c r="F27" s="47">
+        <v>3</v>
+      </c>
       <c r="G27" s="25" t="str">
         <f>AB23</f>
         <v>Argentina</v>
       </c>
-      <c r="H27" s="28"/>
+      <c r="H27" s="28">
+        <v>26</v>
+      </c>
       <c r="I27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J27" s="30"/>
-      <c r="K27" s="28"/>
+      <c r="J27" s="30">
+        <v>28</v>
+      </c>
+      <c r="K27" s="28">
+        <v>23</v>
+      </c>
       <c r="L27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M27" s="30"/>
-      <c r="N27" s="28"/>
+      <c r="M27" s="30">
+        <v>25</v>
+      </c>
+      <c r="N27" s="28">
+        <v>25</v>
+      </c>
       <c r="O27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="28"/>
+      <c r="P27" s="30">
+        <v>21</v>
+      </c>
+      <c r="Q27" s="28">
+        <v>25</v>
+      </c>
       <c r="R27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S27" s="30"/>
-      <c r="T27" s="28"/>
+      <c r="S27" s="30">
+        <v>20</v>
+      </c>
+      <c r="T27" s="28">
+        <v>12</v>
+      </c>
       <c r="U27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="V27" s="30"/>
+      <c r="V27" s="30">
+        <v>15</v>
+      </c>
       <c r="W27" s="31">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="X27" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y27" s="32">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="AD27" s="12">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="AE27" s="12">
+        <v>5</v>
+      </c>
+      <c r="AE27" s="12" t="str">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>Argentina</v>
       </c>
       <c r="AF27" s="12">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG27" s="12">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH27" s="12">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI27" s="12">
         <f t="shared" si="47"/>
@@ -9848,35 +9932,35 @@
       </c>
       <c r="AK27" s="12">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL27" s="12">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="AM27" s="12">
         <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="AO27" s="12">
+        <v>111</v>
+      </c>
+      <c r="AO27" s="12" t="str">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>France</v>
       </c>
       <c r="AP27" s="12">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ27" s="12">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR27" s="12">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS27" s="12">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT27" s="12">
         <f t="shared" si="57"/>
@@ -9888,15 +9972,15 @@
       </c>
       <c r="AV27" s="12">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="AW27" s="12">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="BA27" s="26">
         <f>SUM(BA23:BA26)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13392,15 +13476,15 @@
       </c>
       <c r="AZ47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,3,FALSE)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BA47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BC47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,6,FALSE)</f>
@@ -13408,7 +13492,7 @@
       </c>
       <c r="BD47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,7,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,8,FALSE)</f>
@@ -13432,7 +13516,7 @@
       </c>
       <c r="BJ47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,13,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BK47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,14,FALSE)</f>
@@ -13440,19 +13524,19 @@
       </c>
       <c r="BL47" s="52">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,15,FALSE)</f>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="BM47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,16,FALSE)</f>
-        <v>183</v>
+        <v>258</v>
       </c>
       <c r="BN47" s="50">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,17,FALSE)</f>
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="BO47" s="52">
         <f>VLOOKUP($AX47,Dummy!$B$23:$S$26,18,FALSE)</f>
-        <v>1136.6459627329193</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="48" spans="2:70" x14ac:dyDescent="0.25">
@@ -13615,15 +13699,15 @@
       </c>
       <c r="AZ48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,3,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BA48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,6,FALSE)</f>
@@ -13631,7 +13715,7 @@
       </c>
       <c r="BD48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,7,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,8,FALSE)</f>
@@ -13655,7 +13739,7 @@
       </c>
       <c r="BJ48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,13,FALSE)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="BK48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,14,FALSE)</f>
@@ -13663,19 +13747,19 @@
       </c>
       <c r="BL48" s="52">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,15,FALSE)</f>
-        <v>1666.6666666666667</v>
+        <v>2666.6666666666665</v>
       </c>
       <c r="BM48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,16,FALSE)</f>
-        <v>181</v>
+        <v>256</v>
       </c>
       <c r="BN48" s="50">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,17,FALSE)</f>
-        <v>160</v>
+        <v>221</v>
       </c>
       <c r="BO48" s="52">
         <f>VLOOKUP($AX48,Dummy!$B$23:$S$26,18,FALSE)</f>
-        <v>1131.25</v>
+        <v>1158.3710407239821</v>
       </c>
     </row>
     <row r="49" spans="2:67" x14ac:dyDescent="0.25">
@@ -13850,7 +13934,7 @@
       </c>
       <c r="BA49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,5,FALSE)</f>
@@ -13858,7 +13942,7 @@
       </c>
       <c r="BC49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BD49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,7,FALSE)</f>
@@ -13882,7 +13966,7 @@
       </c>
       <c r="BI49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,12,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BJ49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,13,FALSE)</f>
@@ -13890,23 +13974,23 @@
       </c>
       <c r="BK49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,14,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BL49" s="52">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,15,FALSE)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="BM49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,16,FALSE)</f>
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="BN49" s="50">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,17,FALSE)</f>
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="BO49" s="52">
         <f>VLOOKUP($AX49,Dummy!$B$23:$S$26,18,FALSE)</f>
-        <v>1130.4347826086955</v>
+        <v>1005.2631578947369</v>
       </c>
     </row>
     <row r="50" spans="2:67" x14ac:dyDescent="0.25">
@@ -13917,30 +14001,46 @@
         <f>AB48</f>
         <v>Belgium</v>
       </c>
-      <c r="D50" s="48"/>
+      <c r="D50" s="48">
+        <v>3</v>
+      </c>
       <c r="E50" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F50" s="47"/>
+      <c r="F50" s="47">
+        <v>0</v>
+      </c>
       <c r="G50" s="5" t="str">
         <f>AB49</f>
         <v>Algeria</v>
       </c>
-      <c r="H50" s="28"/>
+      <c r="H50" s="28">
+        <v>25</v>
+      </c>
       <c r="I50" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J50" s="30"/>
-      <c r="K50" s="28"/>
+      <c r="J50" s="30">
+        <v>22</v>
+      </c>
+      <c r="K50" s="28">
+        <v>25</v>
+      </c>
       <c r="L50" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M50" s="30"/>
-      <c r="N50" s="28"/>
+      <c r="M50" s="30">
+        <v>20</v>
+      </c>
+      <c r="N50" s="28">
+        <v>25</v>
+      </c>
       <c r="O50" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P50" s="30"/>
+      <c r="P50" s="30">
+        <v>12</v>
+      </c>
       <c r="Q50" s="28"/>
       <c r="R50" s="29" t="s">
         <v>0</v>
@@ -13953,30 +14053,30 @@
       <c r="V50" s="30"/>
       <c r="W50" s="31">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X50" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y50" s="32">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AD50" s="12">
         <f t="shared" si="105"/>
-        <v>0</v>
-      </c>
-      <c r="AE50" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE50" s="12" t="str">
         <f t="shared" si="106"/>
-        <v>0</v>
+        <v>Belgium</v>
       </c>
       <c r="AF50" s="12">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG50" s="12">
         <f t="shared" si="108"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH50" s="12">
         <f t="shared" si="109"/>
@@ -13984,7 +14084,7 @@
       </c>
       <c r="AI50" s="12">
         <f t="shared" si="110"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ50" s="12">
         <f t="shared" si="111"/>
@@ -13996,19 +14096,19 @@
       </c>
       <c r="AL50" s="12">
         <f t="shared" si="113"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AM50" s="12">
         <f t="shared" si="114"/>
-        <v>0</v>
-      </c>
-      <c r="AO50" s="12">
+        <v>54</v>
+      </c>
+      <c r="AO50" s="12" t="str">
         <f t="shared" si="115"/>
-        <v>0</v>
+        <v>Algeria</v>
       </c>
       <c r="AP50" s="12">
         <f t="shared" si="116"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ50" s="12">
         <f t="shared" si="117"/>
@@ -14016,7 +14116,7 @@
       </c>
       <c r="AR50" s="12">
         <f t="shared" si="118"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS50" s="12">
         <f t="shared" si="119"/>
@@ -14028,15 +14128,15 @@
       </c>
       <c r="AU50" s="12">
         <f t="shared" si="121"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV50" s="12">
         <f t="shared" si="122"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AW50" s="12">
         <f t="shared" si="123"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AX50" s="50">
         <v>4</v>
@@ -14051,7 +14151,7 @@
       </c>
       <c r="BA50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,5,FALSE)</f>
@@ -14059,7 +14159,7 @@
       </c>
       <c r="BC50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,6,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,7,FALSE)</f>
@@ -14083,7 +14183,7 @@
       </c>
       <c r="BI50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,12,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BJ50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,13,FALSE)</f>
@@ -14091,7 +14191,7 @@
       </c>
       <c r="BK50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,14,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BL50" s="52">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,15,FALSE)</f>
@@ -14099,15 +14199,15 @@
       </c>
       <c r="BM50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,16,FALSE)</f>
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="BN50" s="50">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,17,FALSE)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="BO50" s="52">
         <f>VLOOKUP($AX50,Dummy!$B$23:$S$26,18,FALSE)</f>
-        <v>613.33333333333326</v>
+        <v>648.8888888888888</v>
       </c>
     </row>
     <row r="51" spans="2:67" x14ac:dyDescent="0.25">
@@ -14118,30 +14218,46 @@
         <f>AB46</f>
         <v>Italy</v>
       </c>
-      <c r="D51" s="48"/>
+      <c r="D51" s="48">
+        <v>3</v>
+      </c>
       <c r="E51" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F51" s="47"/>
+      <c r="F51" s="47">
+        <v>0</v>
+      </c>
       <c r="G51" s="5" t="str">
         <f>AB47</f>
         <v>Ukraine</v>
       </c>
-      <c r="H51" s="28"/>
+      <c r="H51" s="28">
+        <v>25</v>
+      </c>
       <c r="I51" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J51" s="30"/>
-      <c r="K51" s="28"/>
+      <c r="J51" s="30">
+        <v>21</v>
+      </c>
+      <c r="K51" s="28">
+        <v>25</v>
+      </c>
       <c r="L51" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M51" s="30"/>
-      <c r="N51" s="28"/>
+      <c r="M51" s="30">
+        <v>22</v>
+      </c>
+      <c r="N51" s="28">
+        <v>25</v>
+      </c>
       <c r="O51" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P51" s="30"/>
+      <c r="P51" s="30">
+        <v>18</v>
+      </c>
       <c r="Q51" s="28"/>
       <c r="R51" s="29" t="s">
         <v>0</v>
@@ -14154,30 +14270,30 @@
       <c r="V51" s="30"/>
       <c r="W51" s="31">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X51" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y51" s="32">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="AD51" s="12">
         <f t="shared" si="105"/>
-        <v>0</v>
-      </c>
-      <c r="AE51" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE51" s="12" t="str">
         <f t="shared" si="106"/>
-        <v>0</v>
+        <v>Italy</v>
       </c>
       <c r="AF51" s="12">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG51" s="12">
         <f t="shared" si="108"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH51" s="12">
         <f t="shared" si="109"/>
@@ -14185,7 +14301,7 @@
       </c>
       <c r="AI51" s="12">
         <f t="shared" si="110"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ51" s="12">
         <f t="shared" si="111"/>
@@ -14197,19 +14313,19 @@
       </c>
       <c r="AL51" s="12">
         <f t="shared" si="113"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AM51" s="12">
         <f t="shared" si="114"/>
-        <v>0</v>
-      </c>
-      <c r="AO51" s="12">
+        <v>61</v>
+      </c>
+      <c r="AO51" s="12" t="str">
         <f t="shared" si="115"/>
-        <v>0</v>
+        <v>Ukraine</v>
       </c>
       <c r="AP51" s="12">
         <f t="shared" si="116"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ51" s="12">
         <f t="shared" si="117"/>
@@ -14217,7 +14333,7 @@
       </c>
       <c r="AR51" s="12">
         <f t="shared" si="118"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS51" s="12">
         <f t="shared" si="119"/>
@@ -14229,19 +14345,19 @@
       </c>
       <c r="AU51" s="12">
         <f t="shared" si="121"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV51" s="12">
         <f t="shared" si="122"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="AW51" s="12">
         <f t="shared" si="123"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="BA51" s="26">
         <f>SUM(BA47:BA50)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16254,7 +16370,7 @@
       </c>
       <c r="AY63" s="51" t="str">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,2,FALSE)</f>
-        <v>Brazil</v>
+        <v>Serbia</v>
       </c>
       <c r="AZ63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,3,FALSE)</f>
@@ -16262,7 +16378,7 @@
       </c>
       <c r="BA63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,5,FALSE)</f>
@@ -16270,15 +16386,15 @@
       </c>
       <c r="BC63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,7,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,8,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,9,FALSE)</f>
@@ -16294,7 +16410,7 @@
       </c>
       <c r="BI63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,12,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,13,FALSE)</f>
@@ -16302,23 +16418,23 @@
       </c>
       <c r="BK63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,14,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BL63" s="52">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,15,FALSE)</f>
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="BM63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,16,FALSE)</f>
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="BN63" s="50">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,17,FALSE)</f>
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="BO63" s="52">
         <f>VLOOKUP($AX63,Dummy!$B$31:$S$34,18,FALSE)</f>
-        <v>1190.1408450704225</v>
+        <v>1078.8177339901476</v>
       </c>
     </row>
     <row r="64" spans="2:67" x14ac:dyDescent="0.25">
@@ -16477,19 +16593,19 @@
       </c>
       <c r="AY64" s="51" t="str">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,2,FALSE)</f>
-        <v>Serbia</v>
+        <v>Czech Republic</v>
       </c>
       <c r="AZ64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BA64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,6,FALSE)</f>
@@ -16497,7 +16613,7 @@
       </c>
       <c r="BD64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,7,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,8,FALSE)</f>
@@ -16521,7 +16637,7 @@
       </c>
       <c r="BJ64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,13,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BK64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,14,FALSE)</f>
@@ -16529,19 +16645,19 @@
       </c>
       <c r="BL64" s="52">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,15,FALSE)</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="BM64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,16,FALSE)</f>
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="BN64" s="50">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,17,FALSE)</f>
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="BO64" s="52">
         <f>VLOOKUP($AX64,Dummy!$B$31:$S$34,18,FALSE)</f>
-        <v>1035.9712230215828</v>
+        <v>1004.9751243781095</v>
       </c>
     </row>
     <row r="65" spans="2:67" x14ac:dyDescent="0.25">
@@ -16700,19 +16816,19 @@
       </c>
       <c r="AY65" s="51" t="str">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,2,FALSE)</f>
-        <v>Czech Republic</v>
+        <v>Brazil</v>
       </c>
       <c r="AZ65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BA65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BC65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,6,FALSE)</f>
@@ -16724,7 +16840,7 @@
       </c>
       <c r="BE65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,8,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,9,FALSE)</f>
@@ -16744,27 +16860,27 @@
       </c>
       <c r="BJ65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,13,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BK65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,14,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BL65" s="52">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,15,FALSE)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="BM65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,16,FALSE)</f>
-        <v>126</v>
+        <v>233</v>
       </c>
       <c r="BN65" s="50">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,17,FALSE)</f>
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="BO65" s="52">
         <f>VLOOKUP($AX65,Dummy!$B$31:$S$34,18,FALSE)</f>
-        <v>900</v>
+        <v>1073.7327188940092</v>
       </c>
     </row>
     <row r="66" spans="2:67" x14ac:dyDescent="0.25">
@@ -16775,30 +16891,46 @@
         <f>AB64</f>
         <v>Czech Republic</v>
       </c>
-      <c r="D66" s="48"/>
+      <c r="D66" s="48">
+        <v>3</v>
+      </c>
       <c r="E66" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F66" s="47"/>
+      <c r="F66" s="47">
+        <v>0</v>
+      </c>
       <c r="G66" s="5" t="str">
         <f>AB65</f>
         <v>China</v>
       </c>
-      <c r="H66" s="28"/>
+      <c r="H66" s="28">
+        <v>26</v>
+      </c>
       <c r="I66" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J66" s="30"/>
-      <c r="K66" s="28"/>
+      <c r="J66" s="30">
+        <v>24</v>
+      </c>
+      <c r="K66" s="28">
+        <v>25</v>
+      </c>
       <c r="L66" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M66" s="30"/>
-      <c r="N66" s="28"/>
+      <c r="M66" s="30">
+        <v>19</v>
+      </c>
+      <c r="N66" s="28">
+        <v>25</v>
+      </c>
       <c r="O66" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P66" s="30"/>
+      <c r="P66" s="30">
+        <v>18</v>
+      </c>
       <c r="Q66" s="28"/>
       <c r="R66" s="29" t="s">
         <v>0</v>
@@ -16811,30 +16943,30 @@
       <c r="V66" s="30"/>
       <c r="W66" s="31">
         <f t="shared" si="166"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="X66" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y66" s="32">
         <f t="shared" si="167"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="AD66" s="12">
         <f t="shared" si="147"/>
-        <v>0</v>
-      </c>
-      <c r="AE66" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE66" s="12" t="str">
         <f t="shared" si="148"/>
-        <v>0</v>
+        <v>Czech Republic</v>
       </c>
       <c r="AF66" s="12">
         <f t="shared" si="149"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG66" s="12">
         <f t="shared" si="150"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH66" s="12">
         <f t="shared" si="151"/>
@@ -16842,7 +16974,7 @@
       </c>
       <c r="AI66" s="12">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ66" s="12">
         <f t="shared" si="153"/>
@@ -16854,19 +16986,19 @@
       </c>
       <c r="AL66" s="12">
         <f t="shared" si="155"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AM66" s="12">
         <f t="shared" si="156"/>
-        <v>0</v>
-      </c>
-      <c r="AO66" s="12">
+        <v>61</v>
+      </c>
+      <c r="AO66" s="12" t="str">
         <f t="shared" si="157"/>
-        <v>0</v>
+        <v>China</v>
       </c>
       <c r="AP66" s="12">
         <f t="shared" si="158"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ66" s="12">
         <f t="shared" si="159"/>
@@ -16874,7 +17006,7 @@
       </c>
       <c r="AR66" s="12">
         <f t="shared" si="160"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS66" s="12">
         <f t="shared" si="161"/>
@@ -16886,15 +17018,15 @@
       </c>
       <c r="AU66" s="12">
         <f t="shared" si="163"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV66" s="12">
         <f t="shared" si="164"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="AW66" s="12">
         <f t="shared" si="165"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AX66" s="50">
         <v>4</v>
@@ -16909,7 +17041,7 @@
       </c>
       <c r="BA66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,5,FALSE)</f>
@@ -16917,7 +17049,7 @@
       </c>
       <c r="BC66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,6,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,7,FALSE)</f>
@@ -16941,7 +17073,7 @@
       </c>
       <c r="BI66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,12,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BJ66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,13,FALSE)</f>
@@ -16949,23 +17081,23 @@
       </c>
       <c r="BK66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,14,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="BL66" s="52">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,15,FALSE)</f>
-        <v>166.66666666666666</v>
+        <v>111.1111111111111</v>
       </c>
       <c r="BM66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,16,FALSE)</f>
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="BN66" s="50">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,17,FALSE)</f>
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="BO66" s="52">
         <f>VLOOKUP($AX66,Dummy!$B$31:$S$34,18,FALSE)</f>
-        <v>895.95375722543361</v>
+        <v>867.46987951807228</v>
       </c>
     </row>
     <row r="67" spans="2:67" x14ac:dyDescent="0.25">
@@ -16976,30 +17108,46 @@
         <f>AB62</f>
         <v>Brazil</v>
       </c>
-      <c r="D67" s="48"/>
+      <c r="D67" s="48">
+        <v>0</v>
+      </c>
       <c r="E67" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F67" s="47"/>
+      <c r="F67" s="47">
+        <v>3</v>
+      </c>
       <c r="G67" s="5" t="str">
         <f>AB63</f>
         <v>Serbia</v>
       </c>
-      <c r="H67" s="28"/>
+      <c r="H67" s="28">
+        <v>22</v>
+      </c>
       <c r="I67" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J67" s="30"/>
-      <c r="K67" s="28"/>
+      <c r="J67" s="30">
+        <v>25</v>
+      </c>
+      <c r="K67" s="28">
+        <v>20</v>
+      </c>
       <c r="L67" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M67" s="30"/>
-      <c r="N67" s="28"/>
+      <c r="M67" s="30">
+        <v>25</v>
+      </c>
+      <c r="N67" s="28">
+        <v>22</v>
+      </c>
       <c r="O67" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P67" s="30"/>
+      <c r="P67" s="30">
+        <v>25</v>
+      </c>
       <c r="Q67" s="28"/>
       <c r="R67" s="29" t="s">
         <v>0</v>
@@ -17012,30 +17160,30 @@
       <c r="V67" s="30"/>
       <c r="W67" s="31">
         <f t="shared" si="166"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="X67" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y67" s="32">
         <f t="shared" si="167"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AD67" s="12">
         <f t="shared" si="147"/>
-        <v>0</v>
-      </c>
-      <c r="AE67" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE67" s="12" t="str">
         <f t="shared" si="148"/>
-        <v>0</v>
+        <v>Serbia</v>
       </c>
       <c r="AF67" s="12">
         <f t="shared" si="149"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG67" s="12">
         <f t="shared" si="150"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH67" s="12">
         <f t="shared" si="151"/>
@@ -17043,7 +17191,7 @@
       </c>
       <c r="AI67" s="12">
         <f t="shared" si="152"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ67" s="12">
         <f t="shared" si="153"/>
@@ -17055,19 +17203,19 @@
       </c>
       <c r="AL67" s="12">
         <f t="shared" si="155"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AM67" s="12">
         <f t="shared" si="156"/>
-        <v>0</v>
-      </c>
-      <c r="AO67" s="12">
+        <v>64</v>
+      </c>
+      <c r="AO67" s="12" t="str">
         <f t="shared" si="157"/>
-        <v>0</v>
+        <v>Brazil</v>
       </c>
       <c r="AP67" s="12">
         <f t="shared" si="158"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ67" s="12">
         <f t="shared" si="159"/>
@@ -17075,7 +17223,7 @@
       </c>
       <c r="AR67" s="12">
         <f t="shared" si="160"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS67" s="12">
         <f t="shared" si="161"/>
@@ -17087,19 +17235,19 @@
       </c>
       <c r="AU67" s="12">
         <f t="shared" si="163"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV67" s="12">
         <f t="shared" si="164"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="AW67" s="12">
         <f t="shared" si="165"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="BA67" s="26">
         <f>SUM(BA63:BA66)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -17553,7 +17701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8907CF4-F9AC-40E8-A2EF-9961349DD93C}">
   <dimension ref="B1:BO48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -17825,7 +17973,7 @@
       </c>
       <c r="C6" s="24" t="str">
         <f>IF(Preliminary!BA7&lt;3,"Winner of Pool A",Preliminary!AY7)</f>
-        <v>Winner of Pool A</v>
+        <v>Tunisia</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="49" t="s">
@@ -17834,7 +17982,7 @@
       <c r="F6" s="47"/>
       <c r="G6" s="25" t="str">
         <f>IF(Preliminary!BA64&lt;3,"Runners-up of Pool H",Preliminary!AY64)</f>
-        <v>Runners-up of Pool H</v>
+        <v>Czech Republic</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="29" t="s">
@@ -17956,7 +18104,7 @@
       </c>
       <c r="C7" s="24" t="str">
         <f>IF(Preliminary!BA63&lt;3,"Winner of Pool H",Preliminary!AY63)</f>
-        <v>Winner of Pool H</v>
+        <v>Serbia</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="49" t="s">
@@ -17965,7 +18113,7 @@
       <c r="F7" s="47"/>
       <c r="G7" s="25" t="str">
         <f>IF(Preliminary!BA8&lt;3,"Runners-up of Pool A",Preliminary!AY8)</f>
-        <v>Runners-up of Pool A</v>
+        <v>Iran</v>
       </c>
       <c r="H7" s="28"/>
       <c r="I7" s="29" t="s">
@@ -18346,7 +18494,7 @@
       </c>
       <c r="C10" s="24" t="str">
         <f>IF(Preliminary!BA23&lt;3,"Winner of Pool C",Preliminary!AY23)</f>
-        <v>Winner of Pool C</v>
+        <v>Argentina</v>
       </c>
       <c r="D10" s="48"/>
       <c r="E10" s="49" t="s">
@@ -18355,7 +18503,7 @@
       <c r="F10" s="47"/>
       <c r="G10" s="25" t="str">
         <f>IF(Preliminary!BA48&lt;3,"Runners-up of Pool F",Preliminary!AY48)</f>
-        <v>Runners-up of Pool F</v>
+        <v>Italy</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="29" t="s">
@@ -18476,7 +18624,7 @@
       </c>
       <c r="C11" s="24" t="str">
         <f>IF(Preliminary!BA47&lt;3,"Winner of Pool F",Preliminary!AY47)</f>
-        <v>Winner of Pool F</v>
+        <v>Belgium</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="49" t="s">
@@ -18485,7 +18633,7 @@
       <c r="F11" s="47"/>
       <c r="G11" s="25" t="str">
         <f>IF(Preliminary!BA24&lt;3,"Runners-up of Pool C",Preliminary!AY24)</f>
-        <v>Runners-up of Pool C</v>
+        <v>Finland</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="29" t="s">
@@ -21189,16 +21337,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>